<commit_message>
Knapsack problem is solved! And I understand how it solve!
</commit_message>
<xml_diff>
--- a/knapsack.xlsx
+++ b/knapsack.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>гитара</t>
   </si>
@@ -58,7 +58,19 @@
 г + н</t>
   </si>
   <si>
-    <t>ноутбук 3 фунта и максимум из 1-фунтового рюкзака</t>
+    <t>IPHONE</t>
+  </si>
+  <si>
+    <t>2000
+I</t>
+  </si>
+  <si>
+    <t>3500
+I + г</t>
+  </si>
+  <si>
+    <t>4000
+I + н</t>
   </si>
 </sst>
 </file>
@@ -402,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D10:K13"/>
+  <dimension ref="D10:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,8 +517,29 @@
       <c r="J13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="4:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>